<commit_message>
fix error on questions
</commit_message>
<xml_diff>
--- a/Questions/animesong.xlsx
+++ b/Questions/animesong.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/My Works/Rails/speedQuizRails/Questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE0E68D-208B-8149-A1F5-94AB772A7BB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BDC12C-9846-F74A-9D24-D459CF8720A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="3100" windowWidth="19200" windowHeight="14900" xr2:uid="{C2EF2DDF-1058-F043-B3EC-FA013CE258A8}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{C2EF2DDF-1058-F043-B3EC-FA013CE258A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
   <si>
     <t>src</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -55,10 +55,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>길크</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>알바뛰는마왕님</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -135,10 +131,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>아이마스 신데마스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>노라가미</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -163,10 +155,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>메이도라, 메이드래곤, 코바야시</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>니세코이</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -183,10 +171,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>카구야</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>마법소녀마도카마기카</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -397,10 +381,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>7G1KkumdUWk</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>startTime</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -493,10 +473,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>러키스타</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>인피니트스트라토스</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -533,6 +509,63 @@
   </si>
   <si>
     <t>에반게리온</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>길크 길티</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>럭키스타</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이마스 신데마스 아이돌마스터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v9iz9glzbMs</t>
+  </si>
+  <si>
+    <t>wT5uF0kAW9Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NUGqGRcNb38</t>
+  </si>
+  <si>
+    <t>49X8c3Q5Ezs</t>
+  </si>
+  <si>
+    <t>카구야 카구야님</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신만세</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엔비</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기교소녀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에망센 에로망가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>바이올렛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메이도라 메이드래곤 코바야시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CFM_zypYFHM</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -908,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C0362E7-04D3-2D49-9AC4-005F7152D7DD}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -923,19 +956,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -943,7 +976,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C2">
         <v>62</v>
@@ -960,16 +993,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C3">
         <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -977,7 +1010,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -986,7 +1019,7 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -994,16 +1027,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C5">
         <v>53</v>
       </c>
       <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
         <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1011,16 +1044,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1028,16 +1061,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C7">
         <v>60</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1045,16 +1078,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
         <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1062,13 +1095,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C9">
         <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1076,13 +1109,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>143</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1090,16 +1123,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C11">
         <v>100</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1107,13 +1140,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1121,13 +1154,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1135,16 +1168,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1152,16 +1185,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C15">
         <v>58</v>
       </c>
       <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" t="s">
         <v>22</v>
-      </c>
-      <c r="E15" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1169,16 +1202,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C16">
         <v>70</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16" t="s">
-        <v>25</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1186,13 +1219,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1200,16 +1233,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1217,16 +1250,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C19">
         <v>100</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1234,16 +1267,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1251,13 +1284,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C21">
         <v>53</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1265,13 +1298,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C22">
         <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1279,16 +1312,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C23">
         <v>51</v>
       </c>
       <c r="D23" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1296,16 +1329,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E24" t="s">
-        <v>37</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1313,16 +1346,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C25">
         <v>50</v>
       </c>
       <c r="D25" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E25" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1330,13 +1363,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C26">
         <v>59</v>
       </c>
       <c r="D26" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+      <c r="E26" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1344,16 +1380,16 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C27">
         <v>109</v>
       </c>
       <c r="D27" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E27" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1361,13 +1397,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C28">
         <v>74</v>
       </c>
       <c r="D28" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1375,13 +1411,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C29">
         <v>73</v>
       </c>
       <c r="D29" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1389,16 +1425,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C30">
         <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E30" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1406,13 +1442,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1420,16 +1456,16 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E32" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1437,16 +1473,16 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E33" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1454,16 +1490,16 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E34" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1471,13 +1507,16 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C35">
         <v>57</v>
       </c>
       <c r="D35" t="s">
-        <v>87</v>
+        <v>83</v>
+      </c>
+      <c r="E35" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1485,16 +1524,16 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C36">
         <v>21</v>
       </c>
       <c r="D36" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E36" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1502,16 +1541,16 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C37">
         <v>14</v>
       </c>
       <c r="D37" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E37" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1519,167 +1558,242 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C38">
         <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:5">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>134</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
       <c r="D39" t="s">
+        <v>98</v>
+      </c>
+      <c r="E39" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>135</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40" t="s">
+        <v>99</v>
+      </c>
+      <c r="E40" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>101</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41" t="s">
+        <v>100</v>
+      </c>
+      <c r="E41" t="s">
         <v>103</v>
       </c>
-      <c r="E39" t="s">
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42" t="s">
+        <v>102</v>
+      </c>
+      <c r="E42" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>116</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43" t="s">
+        <v>115</v>
+      </c>
+      <c r="E43" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="D40" t="s">
-        <v>104</v>
-      </c>
-      <c r="E40" t="s">
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
-      <c r="B41" t="s">
-        <v>106</v>
-      </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
-      <c r="D41" t="s">
-        <v>105</v>
-      </c>
-      <c r="E41" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="B42" t="s">
+    <row r="45" spans="1:5">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>133</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45" t="s">
+        <v>111</v>
+      </c>
+      <c r="E45" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>114</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46" t="s">
         <v>113</v>
       </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-      <c r="D42" t="s">
-        <v>107</v>
-      </c>
-      <c r="E42" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="B43" t="s">
-        <v>121</v>
-      </c>
-      <c r="C43">
-        <v>0</v>
-      </c>
-      <c r="D43" t="s">
-        <v>120</v>
-      </c>
-      <c r="E43" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="B44" t="s">
-        <v>115</v>
-      </c>
-      <c r="C44">
-        <v>0</v>
-      </c>
-      <c r="D44" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="D45" t="s">
-        <v>116</v>
-      </c>
-      <c r="E45" t="s">
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>132</v>
+      </c>
+      <c r="C47">
+        <v>200</v>
+      </c>
+      <c r="D47" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="B46" t="s">
-        <v>119</v>
-      </c>
-      <c r="C46">
-        <v>0</v>
-      </c>
-      <c r="D46" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="D47" t="s">
+      <c r="E47" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="B48" t="s">
-        <v>128</v>
       </c>
       <c r="C48">
         <v>6</v>
       </c>
       <c r="D48" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>120</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49" t="s">
+        <v>118</v>
+      </c>
+      <c r="E49" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
         <v>123</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5">
-      <c r="B49" t="s">
-        <v>126</v>
-      </c>
-      <c r="C49">
-        <v>0</v>
-      </c>
-      <c r="D49" t="s">
-        <v>124</v>
-      </c>
-      <c r="E49" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5">
-      <c r="B50" t="s">
-        <v>129</v>
       </c>
       <c r="C50">
         <v>66</v>
       </c>
       <c r="D50" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5">
+        <v>121</v>
+      </c>
+      <c r="E50" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51">
+        <v>50</v>
+      </c>
       <c r="B51" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C51">
         <v>60</v>
       </c>
       <c r="D51" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5">
+        <v>124</v>
+      </c>
+      <c r="E51" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
+        <v>51</v>
+      </c>
       <c r="B52" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C52">
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E52" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add info coloring && fix some questions
</commit_message>
<xml_diff>
--- a/Questions/animesong.xlsx
+++ b/Questions/animesong.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/My Works/Rails/speedQuizRails/Questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BDC12C-9846-F74A-9D24-D459CF8720A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A711D18-A101-5E40-8241-F22DBB53E130}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{C2EF2DDF-1058-F043-B3EC-FA013CE258A8}"/>
+    <workbookView xWindow="28800" yWindow="3140" windowWidth="19200" windowHeight="14860" xr2:uid="{C2EF2DDF-1058-F043-B3EC-FA013CE258A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -225,19 +225,9 @@
     <t>gyJCjbXzcKc</t>
   </si>
   <si>
-    <t>nIrYjzHAEp0</t>
-  </si>
-  <si>
-    <t>GvPa1qcmKbs</t>
-  </si>
-  <si>
     <t>fvBGhH5D8hc</t>
   </si>
   <si>
-    <t>_IkopJwRDKU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DyQydVTeIf8</t>
   </si>
   <si>
@@ -248,9 +238,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>dlFA0Zq1k2A</t>
-  </si>
-  <si>
     <t>EOKAnomhHRg</t>
   </si>
   <si>
@@ -303,10 +290,6 @@
     <t>uwph0dv9E6U</t>
   </si>
   <si>
-    <t>WZKxCkdhDWU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>OkNvl3fNf5A</t>
   </si>
   <si>
@@ -409,9 +392,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>VFadUtWFsQk</t>
-  </si>
-  <si>
     <t>이누야샤</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -466,9 +446,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>IHqlSoqw6mU</t>
-  </si>
-  <si>
     <t>신만이아는세계</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -516,10 +493,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>럭키스타</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>아이마스 신데마스 아이돌마스터</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -527,10 +500,6 @@
     <t>v9iz9glzbMs</t>
   </si>
   <si>
-    <t>wT5uF0kAW9Y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>NUGqGRcNb38</t>
   </si>
   <si>
@@ -567,6 +536,35 @@
   <si>
     <t>CFM_zypYFHM</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sWMntcz5sGE</t>
+  </si>
+  <si>
+    <t>lBsJLPy34yg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>러키스타</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ymwQI1UckUY</t>
+  </si>
+  <si>
+    <t>D8Xt9oNArwc</t>
+  </si>
+  <si>
+    <t>1cMKPc3Yors</t>
+  </si>
+  <si>
+    <t>ZJ83d7SP4jM</t>
+  </si>
+  <si>
+    <t>M_tGU3OzaVc</t>
+  </si>
+  <si>
+    <t>f9WBBnzuq6U</t>
   </si>
 </sst>
 </file>
@@ -941,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C0362E7-04D3-2D49-9AC4-005F7152D7DD}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -962,13 +960,13 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -999,7 +997,7 @@
         <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E3" t="s">
         <v>17</v>
@@ -1010,16 +1008,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>142</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1027,7 +1025,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>141</v>
       </c>
       <c r="C5">
         <v>53</v>
@@ -1044,7 +1042,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -1061,10 +1059,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>138</v>
       </c>
       <c r="C7">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
@@ -1078,7 +1076,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1095,7 +1093,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C9">
         <v>33</v>
@@ -1109,7 +1107,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C10">
         <v>50</v>
@@ -1123,7 +1121,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="C11">
         <v>100</v>
@@ -1132,7 +1130,7 @@
         <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1140,7 +1138,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1154,7 +1152,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1168,7 +1166,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1185,7 +1183,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C15">
         <v>58</v>
@@ -1202,7 +1200,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C16">
         <v>70</v>
@@ -1211,7 +1209,7 @@
         <v>23</v>
       </c>
       <c r="E16" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1219,7 +1217,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1233,7 +1231,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1250,7 +1248,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C19">
         <v>100</v>
@@ -1267,7 +1265,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -1276,7 +1274,7 @@
         <v>29</v>
       </c>
       <c r="E20" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1284,7 +1282,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C21">
         <v>53</v>
@@ -1298,7 +1296,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C22">
         <v>30</v>
@@ -1312,13 +1310,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C23">
         <v>51</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E23" t="s">
         <v>32</v>
@@ -1329,7 +1327,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1338,7 +1336,7 @@
         <v>33</v>
       </c>
       <c r="E24" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1346,7 +1344,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C25">
         <v>50</v>
@@ -1363,7 +1361,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C26">
         <v>59</v>
@@ -1372,7 +1370,7 @@
         <v>36</v>
       </c>
       <c r="E26" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1380,10 +1378,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>135</v>
       </c>
       <c r="C27">
-        <v>109</v>
+        <v>0</v>
       </c>
       <c r="D27" t="s">
         <v>37</v>
@@ -1397,7 +1395,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C28">
         <v>74</v>
@@ -1411,7 +1409,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C29">
         <v>73</v>
@@ -1425,7 +1423,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C30">
         <v>30</v>
@@ -1442,7 +1440,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -1456,7 +1454,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -1465,7 +1463,7 @@
         <v>44</v>
       </c>
       <c r="E32" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1473,16 +1471,16 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E33" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1490,16 +1488,16 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E34" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1507,16 +1505,16 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C35">
         <v>57</v>
       </c>
       <c r="D35" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E35" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1524,16 +1522,16 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C36">
         <v>21</v>
       </c>
       <c r="D36" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E36" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1541,16 +1539,16 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C37">
         <v>14</v>
       </c>
       <c r="D37" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E37" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1558,13 +1556,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C38">
         <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1572,16 +1570,16 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E39" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1589,16 +1587,16 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E40" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1606,16 +1604,16 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>101</v>
+        <v>143</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E41" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1623,16 +1621,16 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E42" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1640,16 +1638,16 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E43" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1657,13 +1655,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C44">
         <v>0</v>
       </c>
       <c r="D44" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1671,16 +1669,16 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C45">
         <v>0</v>
       </c>
       <c r="D45" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E45" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1688,13 +1686,13 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C46">
         <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1702,16 +1700,16 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C47">
         <v>200</v>
       </c>
       <c r="D47" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="E47" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1719,13 +1717,13 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C48">
         <v>6</v>
       </c>
       <c r="D48" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1733,16 +1731,16 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C49">
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E49" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1750,16 +1748,16 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C50">
         <v>66</v>
       </c>
       <c r="D50" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="E50" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1767,16 +1765,16 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C51">
         <v>60</v>
       </c>
       <c r="D51" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E51" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1784,16 +1782,16 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C52">
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="E52" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add kpop name question
</commit_message>
<xml_diff>
--- a/Questions/animesong.xlsx
+++ b/Questions/animesong.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/My Works/Rails/speedQuizRails/Questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B28BBA-6802-2343-BC52-2DD2840F1F44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452DFF38-CE27-8745-A347-0C556FE29823}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{C2EF2DDF-1058-F043-B3EC-FA013CE258A8}"/>
   </bookViews>
@@ -342,10 +342,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>철혈의오펜스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>알드노아제로</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -366,10 +362,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>철혈 오펜스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>이누야사완결편</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -583,6 +575,14 @@
   </si>
   <si>
     <t>우마루 건어물여동생우마루 우마루짱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>철혈의오펀스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>철혈 오펀스 철혈의오펜스 오펜스</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -961,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C0362E7-04D3-2D49-9AC4-005F7152D7DD}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -996,7 +996,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C2">
         <v>59</v>
@@ -1013,7 +1013,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C3">
         <v>37</v>
@@ -1030,7 +1030,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1039,7 +1039,7 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1047,7 +1047,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C5">
         <v>53</v>
@@ -1056,7 +1056,7 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1081,7 +1081,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1090,7 +1090,7 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1098,7 +1098,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1129,7 +1129,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C10">
         <v>50</v>
@@ -1143,7 +1143,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C11">
         <v>100</v>
@@ -1160,7 +1160,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -1183,7 +1183,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1234,7 +1234,7 @@
         <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1299,7 +1299,7 @@
         <v>27</v>
       </c>
       <c r="E20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1316,7 +1316,7 @@
         <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1338,7 +1338,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C23">
         <v>20</v>
@@ -1364,7 +1364,7 @@
         <v>31</v>
       </c>
       <c r="E24" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1398,7 +1398,7 @@
         <v>34</v>
       </c>
       <c r="E26" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1406,7 +1406,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1482,7 +1482,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -1525,7 +1525,7 @@
         <v>68</v>
       </c>
       <c r="E34" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1542,7 +1542,7 @@
         <v>69</v>
       </c>
       <c r="E35" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1559,7 +1559,7 @@
         <v>70</v>
       </c>
       <c r="E36" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1576,7 +1576,7 @@
         <v>72</v>
       </c>
       <c r="E37" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1598,16 +1598,16 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>82</v>
+        <v>146</v>
       </c>
       <c r="E39" t="s">
-        <v>88</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1615,16 +1615,16 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1632,16 +1632,16 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1649,16 +1649,16 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E42" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1666,16 +1666,16 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C43">
         <v>24</v>
       </c>
       <c r="D43" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E43" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1683,16 +1683,16 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C44">
         <v>0</v>
       </c>
       <c r="D44" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E44" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1700,16 +1700,16 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C45">
         <v>0</v>
       </c>
       <c r="D45" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E45" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1717,16 +1717,16 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C46">
         <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E46" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1734,16 +1734,16 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C47">
         <v>200</v>
       </c>
       <c r="D47" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1751,13 +1751,13 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C48">
         <v>6</v>
       </c>
       <c r="D48" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1765,16 +1765,16 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C49">
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E49" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1782,16 +1782,16 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C50">
         <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E50" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1799,16 +1799,16 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C51">
         <v>60</v>
       </c>
       <c r="D51" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E51" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1816,16 +1816,16 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52" t="s">
+        <v>101</v>
+      </c>
+      <c r="E52" t="s">
         <v>102</v>
-      </c>
-      <c r="C52">
-        <v>0</v>
-      </c>
-      <c r="D52" t="s">
-        <v>103</v>
-      </c>
-      <c r="E52" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>